<commit_message>
dateutil method is mostly working, but lots of edge cases
</commit_message>
<xml_diff>
--- a/data/ddmmyyyy.xlsx
+++ b/data/ddmmyyyy.xlsx
@@ -1494,7 +1494,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.45173</v>
+        <v>0.7296</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1502,7 +1502,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.68832</v>
+        <v>0.52499</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1510,7 +1510,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.90818</v>
+        <v>0.41871</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1518,7 +1518,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.82835</v>
+        <v>0.28152</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1526,7 +1526,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.3459</v>
+        <v>0.5455</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1534,7 +1534,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.4424</v>
+        <v>0.5854</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1542,7 +1542,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.93231</v>
+        <v>0.06303</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1550,7 +1550,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.1891</v>
+        <v>0.63132</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1558,7 +1558,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.85822</v>
+        <v>0.9933</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1566,7 +1566,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.36035</v>
+        <v>0.27558</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1574,7 +1574,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.97062</v>
+        <v>0.87534</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1582,7 +1582,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.59326</v>
+        <v>0.58446</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1590,7 +1590,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.90495</v>
+        <v>0.25099</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1598,7 +1598,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.80103</v>
+        <v>0.69923</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1606,7 +1606,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.25328</v>
+        <v>0.87621</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1614,7 +1614,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.48653</v>
+        <v>0.64872</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1622,7 +1622,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.81617</v>
+        <v>0.79409</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1630,7 +1630,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.72739</v>
+        <v>0.95208</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1638,7 +1638,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.71421</v>
+        <v>0.99757</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1646,7 +1646,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>0.8426900000000001</v>
+        <v>0.1547</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1654,7 +1654,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0.03163</v>
+        <v>0.64075</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1662,7 +1662,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>0.39359</v>
+        <v>0.95688</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1670,7 +1670,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.06848</v>
+        <v>0.13534</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1678,7 +1678,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0.5158700000000001</v>
+        <v>0.18665</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1686,7 +1686,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>0.6306</v>
+        <v>0.83458</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1694,7 +1694,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0.21321</v>
+        <v>0.1381</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1702,7 +1702,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>0.11135</v>
+        <v>0.04508</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1710,7 +1710,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0.00454</v>
+        <v>0.9621</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1718,7 +1718,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>0.3864</v>
+        <v>0.21364</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1726,7 +1726,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0.22946</v>
+        <v>0.15769</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1734,7 +1734,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>0.02565</v>
+        <v>0.8414700000000001</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1742,7 +1742,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>0.49985</v>
+        <v>0.78547</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1750,7 +1750,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>0.2921</v>
+        <v>0.08402999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1758,7 +1758,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>0.40767</v>
+        <v>0.26767</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1766,7 +1766,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>0.5731000000000001</v>
+        <v>0.6287</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1774,7 +1774,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>0.9205</v>
+        <v>0.50118</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1782,7 +1782,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>0.55426</v>
+        <v>0.45708</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1790,7 +1790,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>0.75157</v>
+        <v>0.55562</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1798,7 +1798,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>0.15486</v>
+        <v>0.47681</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1806,7 +1806,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>0.95585</v>
+        <v>0.64977</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1814,7 +1814,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>0.20715</v>
+        <v>0.06693</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1822,7 +1822,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>0.6294999999999999</v>
+        <v>0.26517</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1830,7 +1830,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>0.05487</v>
+        <v>0.91318</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1838,7 +1838,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>0.02654</v>
+        <v>0.601</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1846,7 +1846,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>0.05887</v>
+        <v>0.8487</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1854,7 +1854,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>0.57272</v>
+        <v>0.3147</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1862,7 +1862,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>0.6087</v>
+        <v>0.50901</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1870,7 +1870,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>0.07127</v>
+        <v>0.39269</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1878,7 +1878,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>0.5567</v>
+        <v>0.43407</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1886,7 +1886,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>0.39602</v>
+        <v>0.57723</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1894,7 +1894,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>0.15473</v>
+        <v>0.88727</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1902,7 +1902,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>0.05086</v>
+        <v>0.7871</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1910,7 +1910,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>0.91983</v>
+        <v>0.87742</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1918,7 +1918,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>0.45361</v>
+        <v>0.38144</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1926,7 +1926,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>0.99846</v>
+        <v>0.34907</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1934,7 +1934,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0.32552</v>
+        <v>0.7440600000000001</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1942,7 +1942,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>0.45976</v>
+        <v>0.5179</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1950,7 +1950,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>0.5041</v>
+        <v>0.45581</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1958,7 +1958,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>0.66216</v>
+        <v>0.17773</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1966,7 +1966,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>0.75987</v>
+        <v>0.91284</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1974,7 +1974,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>0.1703</v>
+        <v>0.93149</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1982,7 +1982,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>0.05124</v>
+        <v>0.66034</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1990,7 +1990,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>0.4527</v>
+        <v>0.14033</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1998,7 +1998,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>0.13657</v>
+        <v>0.92723</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2006,7 +2006,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>0.83389</v>
+        <v>0.76881</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2014,7 +2014,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>0.26687</v>
+        <v>0.67842</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2022,7 +2022,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>0.99032</v>
+        <v>0.0215</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2030,7 +2030,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>0.64915</v>
+        <v>0.94273</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2038,7 +2038,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>0.1664</v>
+        <v>0.71522</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -2046,7 +2046,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>0.76658</v>
+        <v>0.9925</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2054,7 +2054,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>0.336</v>
+        <v>0.71318</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2062,7 +2062,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>0.6634</v>
+        <v>0.85354</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2070,7 +2070,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>0.28389</v>
+        <v>0.89723</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -2078,7 +2078,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>0.01893</v>
+        <v>0.66346</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2086,7 +2086,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>0.9792999999999999</v>
+        <v>0.86639</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2094,7 +2094,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>0.99185</v>
+        <v>0.1718</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2102,7 +2102,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>0.05593</v>
+        <v>0.44871</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -2110,7 +2110,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>0.74358</v>
+        <v>0.4713</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -2118,7 +2118,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>0.49751</v>
+        <v>0.20473</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2126,7 +2126,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>0.57324</v>
+        <v>0.26008</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2134,7 +2134,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>0.08726</v>
+        <v>0.29047</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2142,7 +2142,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>0.33088</v>
+        <v>0.07539999999999999</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -2150,7 +2150,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>0.79319</v>
+        <v>0.69198</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2158,7 +2158,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>0.50383</v>
+        <v>0.78768</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -2166,7 +2166,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>0.04803</v>
+        <v>0.72847</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -2174,7 +2174,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>0.7395699999999999</v>
+        <v>0.69298</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2182,7 +2182,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>0.22997</v>
+        <v>0.5877599999999999</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2190,7 +2190,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>0.24306</v>
+        <v>0.6141799999999999</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2198,7 +2198,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>0.49786</v>
+        <v>0.63281</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2206,7 +2206,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>0.74187</v>
+        <v>0.30331</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2214,7 +2214,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>0.44871</v>
+        <v>0.1791</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2222,7 +2222,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>0.51629</v>
+        <v>0.46244</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2230,7 +2230,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>0.43777</v>
+        <v>0.00889</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2238,7 +2238,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>0.07217999999999999</v>
+        <v>0.02856</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2246,7 +2246,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>0.99494</v>
+        <v>0.16095</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2254,7 +2254,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>0.69509</v>
+        <v>0.29805</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2262,7 +2262,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>0.89136</v>
+        <v>0.87252</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2270,7 +2270,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>0.21718</v>
+        <v>0.18963</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2278,7 +2278,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>0.87138</v>
+        <v>0.10656</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2286,7 +2286,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>0.21624</v>
+        <v>0.42235</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2294,7 +2294,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>0.26499</v>
+        <v>0.28971</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2302,7 +2302,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>0.79342</v>
+        <v>0.70652</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2310,7 +2310,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>0.47221</v>
+        <v>0.09597</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2318,7 +2318,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>0.56571</v>
+        <v>0.05938</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2326,7 +2326,7 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>0.07407999999999999</v>
+        <v>0.55205</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2334,7 +2334,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>0.30538</v>
+        <v>0.53669</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2342,7 +2342,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>0.13665</v>
+        <v>0.76678</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2350,7 +2350,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>0.48264</v>
+        <v>0.21871</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2358,7 +2358,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>0.6675</v>
+        <v>0.70292</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2366,7 +2366,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>0.27854</v>
+        <v>0.73819</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2374,7 +2374,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>0.55694</v>
+        <v>0.00817</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2382,7 +2382,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>0.40839</v>
+        <v>0.64308</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2390,7 +2390,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>0.63047</v>
+        <v>0.18384</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2398,7 +2398,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>0.32438</v>
+        <v>0.16475</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2406,7 +2406,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>0.7295700000000001</v>
+        <v>0.81008</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2414,7 +2414,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>0.82748</v>
+        <v>0.17857</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2422,7 +2422,7 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>0.4369</v>
+        <v>0.5370200000000001</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2430,7 +2430,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>0.44531</v>
+        <v>0.42983</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2438,7 +2438,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>0.7805299999999999</v>
+        <v>0.18327</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2446,7 +2446,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>0.2765</v>
+        <v>0.46114</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2454,7 +2454,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>0.74097</v>
+        <v>0.08332000000000001</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2462,7 +2462,7 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>0.96219</v>
+        <v>0.47462</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2470,7 +2470,7 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>0.3806</v>
+        <v>0.39197</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2478,7 +2478,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>0.04278</v>
+        <v>0.00654</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2486,7 +2486,7 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>0.12762</v>
+        <v>0.45534</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2494,7 +2494,7 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>0.46451</v>
+        <v>0.5459000000000001</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2502,7 +2502,7 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>0.20333</v>
+        <v>0.55607</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2510,7 +2510,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>0.03561</v>
+        <v>0.04664</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2518,7 +2518,7 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>0.7730399999999999</v>
+        <v>0.60084</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2526,7 +2526,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>0.75731</v>
+        <v>0.25803</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2534,7 +2534,7 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>0.86757</v>
+        <v>0.5797</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2542,7 +2542,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>0.62219</v>
+        <v>0.8358100000000001</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2550,7 +2550,7 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>0.5183</v>
+        <v>0.6127</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2558,7 +2558,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>0.07228999999999999</v>
+        <v>0.90909</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2566,7 +2566,7 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>0.54809</v>
+        <v>0.6694600000000001</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2574,7 +2574,7 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>0.05819</v>
+        <v>0.47479</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2582,7 +2582,7 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>0.08107</v>
+        <v>0.92349</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2590,7 +2590,7 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>0.31021</v>
+        <v>0.51813</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2598,7 +2598,7 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>0.92894</v>
+        <v>0.26963</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2606,7 +2606,7 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>0.02267</v>
+        <v>0.73204</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2614,7 +2614,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>0.32915</v>
+        <v>0.05177</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2622,7 +2622,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>0.6381</v>
+        <v>0.58758</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2630,7 +2630,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>0.95792</v>
+        <v>0.32593</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2638,7 +2638,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>0.98864</v>
+        <v>0.27862</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2646,7 +2646,7 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>0.50246</v>
+        <v>0.49563</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2654,7 +2654,7 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>0.70317</v>
+        <v>0.75643</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2662,7 +2662,7 @@
         <v>148</v>
       </c>
       <c r="B148">
-        <v>0.1484</v>
+        <v>0.4868</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2670,7 +2670,7 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>0.62329</v>
+        <v>0.47339</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2678,7 +2678,7 @@
         <v>150</v>
       </c>
       <c r="B150">
-        <v>0.27197</v>
+        <v>0.33531</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2686,7 +2686,7 @@
         <v>151</v>
       </c>
       <c r="B151">
-        <v>0.76412</v>
+        <v>0.2444</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2694,7 +2694,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>0.14091</v>
+        <v>0.74949</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2702,7 +2702,7 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>0.38018</v>
+        <v>0.31752</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2710,7 +2710,7 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>0.33102</v>
+        <v>0.94485</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2718,7 +2718,7 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>0.72058</v>
+        <v>0.43326</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2726,7 +2726,7 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>0.29938</v>
+        <v>0.63601</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2734,7 +2734,7 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>0.81511</v>
+        <v>0.50766</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2742,7 +2742,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>0.38386</v>
+        <v>0.92226</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2750,7 +2750,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>0.41272</v>
+        <v>0.22687</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2758,7 +2758,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>0.98809</v>
+        <v>0.52093</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2766,7 +2766,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>0.32165</v>
+        <v>0.02012</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2774,7 +2774,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>0.99691</v>
+        <v>0.74612</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2782,7 +2782,7 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>0.12417</v>
+        <v>0.20218</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2790,7 +2790,7 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>0.4786</v>
+        <v>0.89184</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2798,7 +2798,7 @@
         <v>165</v>
       </c>
       <c r="B165">
-        <v>0.61826</v>
+        <v>0.20963</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2806,7 +2806,7 @@
         <v>166</v>
       </c>
       <c r="B166">
-        <v>0.91737</v>
+        <v>0.79517</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2814,7 +2814,7 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>0.18328</v>
+        <v>0.72004</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2822,7 +2822,7 @@
         <v>168</v>
       </c>
       <c r="B168">
-        <v>0.24818</v>
+        <v>0.39394</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2830,7 +2830,7 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>0.26548</v>
+        <v>0.63706</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2838,7 +2838,7 @@
         <v>170</v>
       </c>
       <c r="B170">
-        <v>0.19143</v>
+        <v>0.24585</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2846,7 +2846,7 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>0.4939</v>
+        <v>0.18417</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2854,7 +2854,7 @@
         <v>172</v>
       </c>
       <c r="B172">
-        <v>0.19718</v>
+        <v>0.3584</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2862,7 +2862,7 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>0.66261</v>
+        <v>0.39297</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2870,7 +2870,7 @@
         <v>174</v>
       </c>
       <c r="B174">
-        <v>0.23928</v>
+        <v>0.98903</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2878,7 +2878,7 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>0.87822</v>
+        <v>0.61969</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2886,7 +2886,7 @@
         <v>176</v>
       </c>
       <c r="B176">
-        <v>0.48291</v>
+        <v>0.93728</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2894,7 +2894,7 @@
         <v>177</v>
       </c>
       <c r="B177">
-        <v>0.99578</v>
+        <v>0.5052</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -2902,7 +2902,7 @@
         <v>178</v>
       </c>
       <c r="B178">
-        <v>0.38935</v>
+        <v>0.58499</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2910,7 +2910,7 @@
         <v>179</v>
       </c>
       <c r="B179">
-        <v>0.45958</v>
+        <v>0.48067</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2918,7 +2918,7 @@
         <v>180</v>
       </c>
       <c r="B180">
-        <v>0.90457</v>
+        <v>0.25879</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2926,7 +2926,7 @@
         <v>181</v>
       </c>
       <c r="B181">
-        <v>0.44029</v>
+        <v>0.7965100000000001</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2934,7 +2934,7 @@
         <v>182</v>
       </c>
       <c r="B182">
-        <v>0.8485</v>
+        <v>0.98822</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2942,7 +2942,7 @@
         <v>183</v>
       </c>
       <c r="B183">
-        <v>0.23508</v>
+        <v>0.97539</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2950,7 +2950,7 @@
         <v>184</v>
       </c>
       <c r="B184">
-        <v>0.173</v>
+        <v>0.59739</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -2958,7 +2958,7 @@
         <v>185</v>
       </c>
       <c r="B185">
-        <v>0.43715</v>
+        <v>0.68543</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -2966,7 +2966,7 @@
         <v>186</v>
       </c>
       <c r="B186">
-        <v>0.91213</v>
+        <v>0.49355</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -2974,7 +2974,7 @@
         <v>187</v>
       </c>
       <c r="B187">
-        <v>0.74591</v>
+        <v>0.94167</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -2982,7 +2982,7 @@
         <v>188</v>
       </c>
       <c r="B188">
-        <v>0.4564</v>
+        <v>0.21695</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -2990,7 +2990,7 @@
         <v>189</v>
       </c>
       <c r="B189">
-        <v>0.90341</v>
+        <v>0.77626</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -2998,7 +2998,7 @@
         <v>190</v>
       </c>
       <c r="B190">
-        <v>0.65595</v>
+        <v>0.34715</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -3006,7 +3006,7 @@
         <v>191</v>
       </c>
       <c r="B191">
-        <v>0.09103</v>
+        <v>0.20143</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -3014,7 +3014,7 @@
         <v>192</v>
       </c>
       <c r="B192">
-        <v>0.79676</v>
+        <v>0.26608</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -3022,7 +3022,7 @@
         <v>193</v>
       </c>
       <c r="B193">
-        <v>0.42785</v>
+        <v>0.5143799999999999</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -3030,7 +3030,7 @@
         <v>194</v>
       </c>
       <c r="B194">
-        <v>0.72925</v>
+        <v>0.04239</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -3038,7 +3038,7 @@
         <v>195</v>
       </c>
       <c r="B195">
-        <v>0.05717</v>
+        <v>0.17552</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -3046,7 +3046,7 @@
         <v>196</v>
       </c>
       <c r="B196">
-        <v>0.41456</v>
+        <v>0.27537</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -3054,7 +3054,7 @@
         <v>197</v>
       </c>
       <c r="B197">
-        <v>0.54044</v>
+        <v>0.94155</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -3062,7 +3062,7 @@
         <v>198</v>
       </c>
       <c r="B198">
-        <v>0.00758</v>
+        <v>0.17912</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -3070,7 +3070,7 @@
         <v>199</v>
       </c>
       <c r="B199">
-        <v>0.43481</v>
+        <v>0.11996</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -3078,7 +3078,7 @@
         <v>200</v>
       </c>
       <c r="B200">
-        <v>0.51527</v>
+        <v>0.42718</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -3086,7 +3086,7 @@
         <v>201</v>
       </c>
       <c r="B201">
-        <v>0.71123</v>
+        <v>0.76601</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -3094,7 +3094,7 @@
         <v>202</v>
       </c>
       <c r="B202">
-        <v>0.86524</v>
+        <v>0.34874</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -3102,7 +3102,7 @@
         <v>203</v>
       </c>
       <c r="B203">
-        <v>0.99581</v>
+        <v>0.76776</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -3110,7 +3110,7 @@
         <v>204</v>
       </c>
       <c r="B204">
-        <v>0.2762</v>
+        <v>0.1718</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -3118,7 +3118,7 @@
         <v>205</v>
       </c>
       <c r="B205">
-        <v>0.24638</v>
+        <v>0.69168</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -3126,7 +3126,7 @@
         <v>206</v>
       </c>
       <c r="B206">
-        <v>0.00804</v>
+        <v>0.91762</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -3134,7 +3134,7 @@
         <v>207</v>
       </c>
       <c r="B207">
-        <v>0.18165</v>
+        <v>0.94117</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -3142,7 +3142,7 @@
         <v>208</v>
       </c>
       <c r="B208">
-        <v>0.1243</v>
+        <v>0.35787</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -3150,7 +3150,7 @@
         <v>209</v>
       </c>
       <c r="B209">
-        <v>0.51347</v>
+        <v>0.38098</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -3158,7 +3158,7 @@
         <v>210</v>
       </c>
       <c r="B210">
-        <v>0.56327</v>
+        <v>0.45154</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -3166,7 +3166,7 @@
         <v>211</v>
       </c>
       <c r="B211">
-        <v>0.7674800000000001</v>
+        <v>0.8358100000000001</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -3174,7 +3174,7 @@
         <v>212</v>
       </c>
       <c r="B212">
-        <v>0.8932099999999999</v>
+        <v>0.07174</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -3182,7 +3182,7 @@
         <v>213</v>
       </c>
       <c r="B213">
-        <v>0.61612</v>
+        <v>0.7525500000000001</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -3190,7 +3190,7 @@
         <v>214</v>
       </c>
       <c r="B214">
-        <v>0.55403</v>
+        <v>0.31099</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -3198,7 +3198,7 @@
         <v>215</v>
       </c>
       <c r="B215">
-        <v>0.29951</v>
+        <v>0.58061</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -3206,7 +3206,7 @@
         <v>216</v>
       </c>
       <c r="B216">
-        <v>0.53501</v>
+        <v>0.5752699999999999</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -3214,7 +3214,7 @@
         <v>217</v>
       </c>
       <c r="B217">
-        <v>0.60692</v>
+        <v>0.87754</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -3222,7 +3222,7 @@
         <v>218</v>
       </c>
       <c r="B218">
-        <v>0.008500000000000001</v>
+        <v>0.61531</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -3230,7 +3230,7 @@
         <v>219</v>
       </c>
       <c r="B219">
-        <v>0.57277</v>
+        <v>0.12582</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -3238,7 +3238,7 @@
         <v>220</v>
       </c>
       <c r="B220">
-        <v>0.33825</v>
+        <v>0.7819700000000001</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -3246,7 +3246,7 @@
         <v>221</v>
       </c>
       <c r="B221">
-        <v>0.85268</v>
+        <v>0.06151</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -3254,7 +3254,7 @@
         <v>222</v>
       </c>
       <c r="B222">
-        <v>0.74466</v>
+        <v>0.12026</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -3262,7 +3262,7 @@
         <v>223</v>
       </c>
       <c r="B223">
-        <v>0.29486</v>
+        <v>0.67865</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -3270,7 +3270,7 @@
         <v>224</v>
       </c>
       <c r="B224">
-        <v>0.23387</v>
+        <v>0.92761</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -3278,7 +3278,7 @@
         <v>225</v>
       </c>
       <c r="B225">
-        <v>0.00827</v>
+        <v>0.64141</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -3286,7 +3286,7 @@
         <v>226</v>
       </c>
       <c r="B226">
-        <v>0.19941</v>
+        <v>0.13943</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -3294,7 +3294,7 @@
         <v>227</v>
       </c>
       <c r="B227">
-        <v>0.047</v>
+        <v>0.01104</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -3302,7 +3302,7 @@
         <v>228</v>
       </c>
       <c r="B228">
-        <v>0.72067</v>
+        <v>0.74217</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -3310,7 +3310,7 @@
         <v>229</v>
       </c>
       <c r="B229">
-        <v>0.95005</v>
+        <v>0.04318</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -3318,7 +3318,7 @@
         <v>230</v>
       </c>
       <c r="B230">
-        <v>0.78807</v>
+        <v>0.33512</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -3326,7 +3326,7 @@
         <v>231</v>
       </c>
       <c r="B231">
-        <v>0.39381</v>
+        <v>0.32076</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -3334,7 +3334,7 @@
         <v>232</v>
       </c>
       <c r="B232">
-        <v>0.59793</v>
+        <v>0.11081</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -3342,7 +3342,7 @@
         <v>233</v>
       </c>
       <c r="B233">
-        <v>0.36428</v>
+        <v>0.23471</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -3350,7 +3350,7 @@
         <v>234</v>
       </c>
       <c r="B234">
-        <v>0.45406</v>
+        <v>0.87335</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -3358,7 +3358,7 @@
         <v>235</v>
       </c>
       <c r="B235">
-        <v>0.06554</v>
+        <v>0.31226</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -3366,7 +3366,7 @@
         <v>236</v>
       </c>
       <c r="B236">
-        <v>0.91092</v>
+        <v>0.40863</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -3374,7 +3374,7 @@
         <v>237</v>
       </c>
       <c r="B237">
-        <v>0.80696</v>
+        <v>0.35537</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -3382,7 +3382,7 @@
         <v>238</v>
       </c>
       <c r="B238">
-        <v>0.04603</v>
+        <v>0.20246</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -3390,7 +3390,7 @@
         <v>239</v>
       </c>
       <c r="B239">
-        <v>0.59774</v>
+        <v>0.11274</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -3398,7 +3398,7 @@
         <v>240</v>
       </c>
       <c r="B240">
-        <v>0.7527</v>
+        <v>0.05262</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -3406,7 +3406,7 @@
         <v>241</v>
       </c>
       <c r="B241">
-        <v>0.25419</v>
+        <v>0.52166</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -3414,7 +3414,7 @@
         <v>242</v>
       </c>
       <c r="B242">
-        <v>0.25141</v>
+        <v>0.28956</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -3422,7 +3422,7 @@
         <v>243</v>
       </c>
       <c r="B243">
-        <v>0.05398</v>
+        <v>0.73638</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -3430,7 +3430,7 @@
         <v>244</v>
       </c>
       <c r="B244">
-        <v>0.3129</v>
+        <v>0.97973</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -3438,7 +3438,7 @@
         <v>245</v>
       </c>
       <c r="B245">
-        <v>0.45226</v>
+        <v>0.73791</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -3446,7 +3446,7 @@
         <v>246</v>
       </c>
       <c r="B246">
-        <v>0.5312</v>
+        <v>0.66679</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -3454,7 +3454,7 @@
         <v>247</v>
       </c>
       <c r="B247">
-        <v>0.68973</v>
+        <v>0.14167</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -3462,7 +3462,7 @@
         <v>248</v>
       </c>
       <c r="B248">
-        <v>0.05459</v>
+        <v>0.93832</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -3470,7 +3470,7 @@
         <v>249</v>
       </c>
       <c r="B249">
-        <v>0.11855</v>
+        <v>0.03802</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -3478,7 +3478,7 @@
         <v>250</v>
       </c>
       <c r="B250">
-        <v>0.5774899999999999</v>
+        <v>0.73564</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -3486,7 +3486,7 @@
         <v>251</v>
       </c>
       <c r="B251">
-        <v>0.61045</v>
+        <v>0.73766</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -3494,7 +3494,7 @@
         <v>252</v>
       </c>
       <c r="B252">
-        <v>0.52684</v>
+        <v>0.99151</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -3502,7 +3502,7 @@
         <v>253</v>
       </c>
       <c r="B253">
-        <v>0.59534</v>
+        <v>0.65126</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -3510,7 +3510,7 @@
         <v>254</v>
       </c>
       <c r="B254">
-        <v>0.00649</v>
+        <v>0.3457</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -3518,7 +3518,7 @@
         <v>255</v>
       </c>
       <c r="B255">
-        <v>0.5208700000000001</v>
+        <v>0.32485</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -3526,7 +3526,7 @@
         <v>256</v>
       </c>
       <c r="B256">
-        <v>0.22241</v>
+        <v>0.02006</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -3534,7 +3534,7 @@
         <v>257</v>
       </c>
       <c r="B257">
-        <v>0.5579499999999999</v>
+        <v>0.54236</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -3542,7 +3542,7 @@
         <v>258</v>
       </c>
       <c r="B258">
-        <v>0.41357</v>
+        <v>0.6398200000000001</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -3550,7 +3550,7 @@
         <v>259</v>
       </c>
       <c r="B259">
-        <v>0.23695</v>
+        <v>0.55171</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -3558,7 +3558,7 @@
         <v>260</v>
       </c>
       <c r="B260">
-        <v>0.36867</v>
+        <v>0.99298</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -3566,7 +3566,7 @@
         <v>261</v>
       </c>
       <c r="B261">
-        <v>0.68106</v>
+        <v>0.69289</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -3574,7 +3574,7 @@
         <v>262</v>
       </c>
       <c r="B262">
-        <v>0.8490799999999999</v>
+        <v>0.28889</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -3582,7 +3582,7 @@
         <v>263</v>
       </c>
       <c r="B263">
-        <v>0.63071</v>
+        <v>0.47502</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -3590,7 +3590,7 @@
         <v>264</v>
       </c>
       <c r="B264">
-        <v>0.6015200000000001</v>
+        <v>0.42204</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -3598,7 +3598,7 @@
         <v>265</v>
       </c>
       <c r="B265">
-        <v>0.9222900000000001</v>
+        <v>0.90524</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -3606,7 +3606,7 @@
         <v>266</v>
       </c>
       <c r="B266">
-        <v>0.7138600000000001</v>
+        <v>0.83739</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -3614,7 +3614,7 @@
         <v>267</v>
       </c>
       <c r="B267">
-        <v>0.8310999999999999</v>
+        <v>0.34902</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -3622,7 +3622,7 @@
         <v>268</v>
       </c>
       <c r="B268">
-        <v>0.49451</v>
+        <v>0.00651</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -3630,7 +3630,7 @@
         <v>269</v>
       </c>
       <c r="B269">
-        <v>0.2951</v>
+        <v>0.03341</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -3638,7 +3638,7 @@
         <v>270</v>
       </c>
       <c r="B270">
-        <v>0.5256</v>
+        <v>0.66952</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -3646,7 +3646,7 @@
         <v>271</v>
       </c>
       <c r="B271">
-        <v>0.83869</v>
+        <v>0.67494</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -3654,7 +3654,7 @@
         <v>272</v>
       </c>
       <c r="B272">
-        <v>0.68275</v>
+        <v>0.16976</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -3662,7 +3662,7 @@
         <v>273</v>
       </c>
       <c r="B273">
-        <v>0.24432</v>
+        <v>0.36312</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -3670,7 +3670,7 @@
         <v>274</v>
       </c>
       <c r="B274">
-        <v>0.83397</v>
+        <v>0.10688</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -3678,7 +3678,7 @@
         <v>275</v>
       </c>
       <c r="B275">
-        <v>0.26061</v>
+        <v>0.8213200000000001</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -3686,7 +3686,7 @@
         <v>276</v>
       </c>
       <c r="B276">
-        <v>0.63247</v>
+        <v>0.64155</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -3694,7 +3694,7 @@
         <v>277</v>
       </c>
       <c r="B277">
-        <v>0.7644300000000001</v>
+        <v>0.61182</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -3702,7 +3702,7 @@
         <v>278</v>
       </c>
       <c r="B278">
-        <v>0.79154</v>
+        <v>0.26261</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -3710,7 +3710,7 @@
         <v>279</v>
       </c>
       <c r="B279">
-        <v>0.50017</v>
+        <v>0.30669</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -3718,7 +3718,7 @@
         <v>280</v>
       </c>
       <c r="B280">
-        <v>0.27898</v>
+        <v>0.12562</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -3726,7 +3726,7 @@
         <v>281</v>
       </c>
       <c r="B281">
-        <v>0.6702</v>
+        <v>0.7412300000000001</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -3734,7 +3734,7 @@
         <v>282</v>
       </c>
       <c r="B282">
-        <v>0.82323</v>
+        <v>0.30973</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -3742,7 +3742,7 @@
         <v>283</v>
       </c>
       <c r="B283">
-        <v>0.83484</v>
+        <v>0.4187</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -3750,7 +3750,7 @@
         <v>284</v>
       </c>
       <c r="B284">
-        <v>0.47862</v>
+        <v>0.19174</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -3758,7 +3758,7 @@
         <v>285</v>
       </c>
       <c r="B285">
-        <v>0.82644</v>
+        <v>0.02241</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -3766,7 +3766,7 @@
         <v>286</v>
       </c>
       <c r="B286">
-        <v>0.05175</v>
+        <v>0.17654</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -3774,7 +3774,7 @@
         <v>287</v>
       </c>
       <c r="B287">
-        <v>0.05506</v>
+        <v>0.53586</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -3782,7 +3782,7 @@
         <v>288</v>
       </c>
       <c r="B288">
-        <v>0.62573</v>
+        <v>0.14333</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -3790,7 +3790,7 @@
         <v>289</v>
       </c>
       <c r="B289">
-        <v>0.7430600000000001</v>
+        <v>0.04201</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -3798,7 +3798,7 @@
         <v>290</v>
       </c>
       <c r="B290">
-        <v>0.74561</v>
+        <v>0.55098</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -3806,7 +3806,7 @@
         <v>291</v>
       </c>
       <c r="B291">
-        <v>0.26831</v>
+        <v>0.2493</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -3814,7 +3814,7 @@
         <v>292</v>
       </c>
       <c r="B292">
-        <v>0.40757</v>
+        <v>0.26564</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -3822,7 +3822,7 @@
         <v>293</v>
       </c>
       <c r="B293">
-        <v>0.79808</v>
+        <v>0.72589</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -3830,7 +3830,7 @@
         <v>294</v>
       </c>
       <c r="B294">
-        <v>0.45829</v>
+        <v>0.8988</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -3838,7 +3838,7 @@
         <v>295</v>
       </c>
       <c r="B295">
-        <v>0.8112</v>
+        <v>0.97798</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -3846,7 +3846,7 @@
         <v>296</v>
       </c>
       <c r="B296">
-        <v>0.16209</v>
+        <v>0.8027300000000001</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -3854,7 +3854,7 @@
         <v>297</v>
       </c>
       <c r="B297">
-        <v>0.70903</v>
+        <v>0.5131599999999999</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -3862,7 +3862,7 @@
         <v>298</v>
       </c>
       <c r="B298">
-        <v>0.26388</v>
+        <v>0.06952999999999999</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -3870,7 +3870,7 @@
         <v>299</v>
       </c>
       <c r="B299">
-        <v>0.89633</v>
+        <v>0.08543000000000001</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -3878,7 +3878,7 @@
         <v>300</v>
       </c>
       <c r="B300">
-        <v>0.86291</v>
+        <v>0.91315</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -3886,7 +3886,7 @@
         <v>301</v>
       </c>
       <c r="B301">
-        <v>0.33565</v>
+        <v>0.71524</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -3894,7 +3894,7 @@
         <v>302</v>
       </c>
       <c r="B302">
-        <v>0.04775</v>
+        <v>0.59797</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -3902,7 +3902,7 @@
         <v>303</v>
       </c>
       <c r="B303">
-        <v>0.34132</v>
+        <v>0.28354</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -3910,7 +3910,7 @@
         <v>304</v>
       </c>
       <c r="B304">
-        <v>0.70388</v>
+        <v>0.35882</v>
       </c>
     </row>
     <row r="305" spans="1:2">
@@ -3918,7 +3918,7 @@
         <v>305</v>
       </c>
       <c r="B305">
-        <v>0.36579</v>
+        <v>0.47296</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -3926,7 +3926,7 @@
         <v>306</v>
       </c>
       <c r="B306">
-        <v>0.32793</v>
+        <v>0.92241</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -3934,7 +3934,7 @@
         <v>307</v>
       </c>
       <c r="B307">
-        <v>0.55747</v>
+        <v>0.10996</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -3942,7 +3942,7 @@
         <v>308</v>
       </c>
       <c r="B308">
-        <v>0.50243</v>
+        <v>0.64477</v>
       </c>
     </row>
     <row r="309" spans="1:2">
@@ -3950,7 +3950,7 @@
         <v>309</v>
       </c>
       <c r="B309">
-        <v>0.78425</v>
+        <v>0.70135</v>
       </c>
     </row>
     <row r="310" spans="1:2">
@@ -3958,7 +3958,7 @@
         <v>310</v>
       </c>
       <c r="B310">
-        <v>0.87464</v>
+        <v>0.93125</v>
       </c>
     </row>
     <row r="311" spans="1:2">
@@ -3966,7 +3966,7 @@
         <v>311</v>
       </c>
       <c r="B311">
-        <v>0.982</v>
+        <v>0.90368</v>
       </c>
     </row>
     <row r="312" spans="1:2">
@@ -3974,7 +3974,7 @@
         <v>312</v>
       </c>
       <c r="B312">
-        <v>0.11846</v>
+        <v>0.9898400000000001</v>
       </c>
     </row>
     <row r="313" spans="1:2">
@@ -3982,7 +3982,7 @@
         <v>313</v>
       </c>
       <c r="B313">
-        <v>0.84195</v>
+        <v>0.22694</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -3990,7 +3990,7 @@
         <v>314</v>
       </c>
       <c r="B314">
-        <v>0.80586</v>
+        <v>0.57753</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -3998,7 +3998,7 @@
         <v>315</v>
       </c>
       <c r="B315">
-        <v>0.88151</v>
+        <v>0.4577</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -4006,7 +4006,7 @@
         <v>316</v>
       </c>
       <c r="B316">
-        <v>0.34974</v>
+        <v>0.70109</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -4014,7 +4014,7 @@
         <v>317</v>
       </c>
       <c r="B317">
-        <v>0.74139</v>
+        <v>0.76888</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -4022,7 +4022,7 @@
         <v>318</v>
       </c>
       <c r="B318">
-        <v>0.54995</v>
+        <v>0.45542</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -4030,7 +4030,7 @@
         <v>319</v>
       </c>
       <c r="B319">
-        <v>0.58005</v>
+        <v>0.58879</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -4038,7 +4038,7 @@
         <v>320</v>
       </c>
       <c r="B320">
-        <v>0.49834</v>
+        <v>0.5096000000000001</v>
       </c>
     </row>
     <row r="321" spans="1:2">
@@ -4046,7 +4046,7 @@
         <v>321</v>
       </c>
       <c r="B321">
-        <v>0.72238</v>
+        <v>0.91064</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -4054,7 +4054,7 @@
         <v>322</v>
       </c>
       <c r="B322">
-        <v>0.97489</v>
+        <v>0.75974</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -4062,7 +4062,7 @@
         <v>323</v>
       </c>
       <c r="B323">
-        <v>0.29594</v>
+        <v>0.2287</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -4070,7 +4070,7 @@
         <v>324</v>
       </c>
       <c r="B324">
-        <v>0.6635799999999999</v>
+        <v>0.07003</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -4078,7 +4078,7 @@
         <v>325</v>
       </c>
       <c r="B325">
-        <v>0.21242</v>
+        <v>0.79332</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -4086,7 +4086,7 @@
         <v>326</v>
       </c>
       <c r="B326">
-        <v>0.5118200000000001</v>
+        <v>0.97299</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -4094,7 +4094,7 @@
         <v>327</v>
       </c>
       <c r="B327">
-        <v>0.29665</v>
+        <v>0.70666</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -4102,7 +4102,7 @@
         <v>328</v>
       </c>
       <c r="B328">
-        <v>0.20831</v>
+        <v>0.32203</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -4110,7 +4110,7 @@
         <v>329</v>
       </c>
       <c r="B329">
-        <v>0.15511</v>
+        <v>0.8082</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -4118,7 +4118,7 @@
         <v>330</v>
       </c>
       <c r="B330">
-        <v>0.9095800000000001</v>
+        <v>0.7325700000000001</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -4126,7 +4126,7 @@
         <v>331</v>
       </c>
       <c r="B331">
-        <v>0.57267</v>
+        <v>0.15973</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -4134,7 +4134,7 @@
         <v>332</v>
       </c>
       <c r="B332">
-        <v>0.20901</v>
+        <v>0.98442</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -4142,7 +4142,7 @@
         <v>333</v>
       </c>
       <c r="B333">
-        <v>0.66259</v>
+        <v>0.1275</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -4150,7 +4150,7 @@
         <v>334</v>
       </c>
       <c r="B334">
-        <v>0.38054</v>
+        <v>0.74988</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -4158,7 +4158,7 @@
         <v>335</v>
       </c>
       <c r="B335">
-        <v>0.34717</v>
+        <v>0.68976</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -4166,7 +4166,7 @@
         <v>336</v>
       </c>
       <c r="B336">
-        <v>0.20294</v>
+        <v>0.68446</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -4174,7 +4174,7 @@
         <v>337</v>
       </c>
       <c r="B337">
-        <v>0.36647</v>
+        <v>0.55413</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -4182,7 +4182,7 @@
         <v>338</v>
       </c>
       <c r="B338">
-        <v>0.50026</v>
+        <v>0.34303</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -4190,7 +4190,7 @@
         <v>339</v>
       </c>
       <c r="B339">
-        <v>0.01196</v>
+        <v>0.85401</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -4198,7 +4198,7 @@
         <v>340</v>
       </c>
       <c r="B340">
-        <v>0.08536000000000001</v>
+        <v>0.13238</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -4206,7 +4206,7 @@
         <v>341</v>
       </c>
       <c r="B341">
-        <v>0.94928</v>
+        <v>0.72238</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -4214,7 +4214,7 @@
         <v>342</v>
       </c>
       <c r="B342">
-        <v>0.34603</v>
+        <v>0.54247</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -4222,7 +4222,7 @@
         <v>343</v>
       </c>
       <c r="B343">
-        <v>0.06117</v>
+        <v>0.18773</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -4230,7 +4230,7 @@
         <v>344</v>
       </c>
       <c r="B344">
-        <v>0.37942</v>
+        <v>0.84635</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -4238,7 +4238,7 @@
         <v>345</v>
       </c>
       <c r="B345">
-        <v>0.53534</v>
+        <v>0.52928</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -4246,7 +4246,7 @@
         <v>346</v>
       </c>
       <c r="B346">
-        <v>0.01532</v>
+        <v>0.9523</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -4254,7 +4254,7 @@
         <v>347</v>
       </c>
       <c r="B347">
-        <v>0.28576</v>
+        <v>0.19798</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -4262,7 +4262,7 @@
         <v>348</v>
       </c>
       <c r="B348">
-        <v>0.56313</v>
+        <v>0.6954900000000001</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -4270,7 +4270,7 @@
         <v>349</v>
       </c>
       <c r="B349">
-        <v>0.51461</v>
+        <v>0.27003</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -4278,7 +4278,7 @@
         <v>350</v>
       </c>
       <c r="B350">
-        <v>0.47712</v>
+        <v>0.16248</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -4286,7 +4286,7 @@
         <v>351</v>
       </c>
       <c r="B351">
-        <v>0.5504</v>
+        <v>0.27852</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -4294,7 +4294,7 @@
         <v>352</v>
       </c>
       <c r="B352">
-        <v>0.24635</v>
+        <v>0.15735</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -4302,7 +4302,7 @@
         <v>353</v>
       </c>
       <c r="B353">
-        <v>0.56434</v>
+        <v>0.48375</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -4310,7 +4310,7 @@
         <v>354</v>
       </c>
       <c r="B354">
-        <v>0.72802</v>
+        <v>0.3623</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -4318,7 +4318,7 @@
         <v>355</v>
       </c>
       <c r="B355">
-        <v>0.4535</v>
+        <v>0.32227</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -4326,7 +4326,7 @@
         <v>356</v>
       </c>
       <c r="B356">
-        <v>0.51052</v>
+        <v>0.51632</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -4334,7 +4334,7 @@
         <v>357</v>
       </c>
       <c r="B357">
-        <v>0.6348200000000001</v>
+        <v>0.58236</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -4342,7 +4342,7 @@
         <v>358</v>
       </c>
       <c r="B358">
-        <v>0.23875</v>
+        <v>0.60898</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -4350,7 +4350,7 @@
         <v>359</v>
       </c>
       <c r="B359">
-        <v>0.71748</v>
+        <v>0.9095299999999999</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -4358,7 +4358,7 @@
         <v>360</v>
       </c>
       <c r="B360">
-        <v>0.03953</v>
+        <v>0.78359</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -4366,7 +4366,7 @@
         <v>361</v>
       </c>
       <c r="B361">
-        <v>0.2351</v>
+        <v>0.78149</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -4374,7 +4374,7 @@
         <v>362</v>
       </c>
       <c r="B362">
-        <v>0.92055</v>
+        <v>0.32916</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -4382,7 +4382,7 @@
         <v>363</v>
       </c>
       <c r="B363">
-        <v>0.75869</v>
+        <v>0.57023</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -4390,7 +4390,7 @@
         <v>364</v>
       </c>
       <c r="B364">
-        <v>0.51512</v>
+        <v>0.10918</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -4398,7 +4398,7 @@
         <v>365</v>
       </c>
       <c r="B365">
-        <v>0.41553</v>
+        <v>0.34749</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -4406,7 +4406,7 @@
         <v>366</v>
       </c>
       <c r="B366">
-        <v>0.61094</v>
+        <v>0.61255</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -4414,7 +4414,7 @@
         <v>367</v>
       </c>
       <c r="B367">
-        <v>0.29656</v>
+        <v>0.22952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>